<commit_message>
Change biogas reactor sampletype
</commit_message>
<xml_diff>
--- a/data/ontology/2025-02-11_mfd-habitat-ontology.xlsx
+++ b/data/ontology/2025-02-11_mfd-habitat-ontology.xlsx
@@ -850,6 +850,39 @@
     <t xml:space="preserve">Activated sludge</t>
   </si>
   <si>
+    <t xml:space="preserve">Drinking water</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tap water</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Waterworks stage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uncleaned/raw water</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Filtered water</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Treated water</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Leachate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Free-living; Saline</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Free-living; Non-saline</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enrichment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">High chalk concentration (limestone quarry)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Biogas</t>
   </si>
   <si>
@@ -860,39 +893,6 @@
   </si>
   <si>
     <t xml:space="preserve">Biogas unknown</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Drinking water</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tap water</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Waterworks stage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Uncleaned/raw water</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Filtered water</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Treated water</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Leachate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Free-living; Saline</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Free-living; Non-saline</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Enrichment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">High chalk concentration (limestone quarry)</t>
   </si>
 </sst>
 </file>
@@ -1008,7 +1008,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1070,10 +1070,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1260,15 +1256,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K282"/>
+  <dimension ref="A1:K1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A231" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K252" activeCellId="0" sqref="K252"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A243" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C277" activeCellId="0" sqref="C277"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="13.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="10.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="27.23"/>
@@ -8901,14 +8897,14 @@
         <v>195</v>
       </c>
       <c r="C255" s="13" t="n">
-        <v>4000</v>
-      </c>
-      <c r="D255" s="13" t="s">
+        <v>3000</v>
+      </c>
+      <c r="D255" s="15" t="s">
         <v>276</v>
       </c>
-      <c r="E255" s="13"/>
-      <c r="F255" s="13"/>
-      <c r="I255" s="13"/>
+      <c r="K255" s="1" t="s">
+        <v>268</v>
+      </c>
     </row>
     <row r="256" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A256" s="13" t="s">
@@ -8918,18 +8914,23 @@
         <v>195</v>
       </c>
       <c r="C256" s="13" t="n">
-        <v>4000</v>
-      </c>
-      <c r="D256" s="13" t="s">
+        <v>3000</v>
+      </c>
+      <c r="D256" s="15" t="s">
         <v>276</v>
       </c>
-      <c r="E256" s="13" t="n">
-        <v>4100</v>
-      </c>
-      <c r="F256" s="13" t="s">
+      <c r="E256" s="15" t="n">
+        <v>3300</v>
+      </c>
+      <c r="F256" s="15" t="s">
         <v>277</v>
       </c>
-      <c r="I256" s="13"/>
+      <c r="G256" s="15"/>
+      <c r="H256" s="15"/>
+      <c r="I256" s="15"/>
+      <c r="K256" s="1" t="s">
+        <v>268</v>
+      </c>
     </row>
     <row r="257" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A257" s="13" t="s">
@@ -8939,18 +8940,23 @@
         <v>195</v>
       </c>
       <c r="C257" s="13" t="n">
-        <v>4000</v>
-      </c>
-      <c r="D257" s="13" t="s">
+        <v>3000</v>
+      </c>
+      <c r="D257" s="15" t="s">
         <v>276</v>
       </c>
-      <c r="E257" s="13" t="n">
-        <v>4200</v>
-      </c>
-      <c r="F257" s="13" t="s">
+      <c r="E257" s="15" t="n">
+        <v>3100</v>
+      </c>
+      <c r="F257" s="15" t="s">
         <v>278</v>
       </c>
-      <c r="I257" s="13"/>
+      <c r="G257" s="15"/>
+      <c r="H257" s="15"/>
+      <c r="I257" s="15"/>
+      <c r="K257" s="1" t="s">
+        <v>268</v>
+      </c>
     </row>
     <row r="258" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A258" s="13" t="s">
@@ -8960,18 +8966,27 @@
         <v>195</v>
       </c>
       <c r="C258" s="13" t="n">
-        <v>4000</v>
-      </c>
-      <c r="D258" s="13" t="s">
+        <v>3000</v>
+      </c>
+      <c r="D258" s="15" t="s">
         <v>276</v>
       </c>
-      <c r="E258" s="13" t="n">
-        <v>4300</v>
-      </c>
-      <c r="F258" s="13" t="s">
+      <c r="E258" s="15" t="n">
+        <v>3100</v>
+      </c>
+      <c r="F258" s="15" t="s">
+        <v>278</v>
+      </c>
+      <c r="G258" s="15" t="n">
+        <v>3110</v>
+      </c>
+      <c r="H258" s="15" t="s">
         <v>279</v>
       </c>
-      <c r="I258" s="13"/>
+      <c r="I258" s="15"/>
+      <c r="K258" s="1" t="s">
+        <v>268</v>
+      </c>
     </row>
     <row r="259" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A259" s="13" t="s">
@@ -8984,8 +8999,21 @@
         <v>3000</v>
       </c>
       <c r="D259" s="15" t="s">
-        <v>280</v>
-      </c>
+        <v>276</v>
+      </c>
+      <c r="E259" s="15" t="n">
+        <v>3100</v>
+      </c>
+      <c r="F259" s="15" t="s">
+        <v>278</v>
+      </c>
+      <c r="G259" s="15" t="n">
+        <v>3120</v>
+      </c>
+      <c r="H259" s="15" t="s">
+        <v>272</v>
+      </c>
+      <c r="I259" s="15"/>
       <c r="K259" s="1" t="s">
         <v>268</v>
       </c>
@@ -9001,16 +9029,20 @@
         <v>3000</v>
       </c>
       <c r="D260" s="15" t="s">
+        <v>276</v>
+      </c>
+      <c r="E260" s="15" t="n">
+        <v>3100</v>
+      </c>
+      <c r="F260" s="15" t="s">
+        <v>278</v>
+      </c>
+      <c r="G260" s="15" t="n">
+        <v>3130</v>
+      </c>
+      <c r="H260" s="15" t="s">
         <v>280</v>
       </c>
-      <c r="E260" s="15" t="n">
-        <v>3300</v>
-      </c>
-      <c r="F260" s="15" t="s">
-        <v>281</v>
-      </c>
-      <c r="G260" s="15"/>
-      <c r="H260" s="15"/>
       <c r="I260" s="15"/>
       <c r="K260" s="1" t="s">
         <v>268</v>
@@ -9027,16 +9059,20 @@
         <v>3000</v>
       </c>
       <c r="D261" s="15" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="E261" s="15" t="n">
         <v>3100</v>
       </c>
       <c r="F261" s="15" t="s">
-        <v>282</v>
-      </c>
-      <c r="G261" s="15"/>
-      <c r="H261" s="15"/>
+        <v>278</v>
+      </c>
+      <c r="G261" s="15" t="n">
+        <v>3140</v>
+      </c>
+      <c r="H261" s="15" t="s">
+        <v>281</v>
+      </c>
       <c r="I261" s="15"/>
       <c r="K261" s="1" t="s">
         <v>268</v>
@@ -9050,24 +9086,14 @@
         <v>195</v>
       </c>
       <c r="C262" s="13" t="n">
-        <v>3000</v>
-      </c>
-      <c r="D262" s="15" t="s">
-        <v>280</v>
-      </c>
-      <c r="E262" s="15" t="n">
-        <v>3100</v>
-      </c>
-      <c r="F262" s="15" t="s">
-        <v>282</v>
-      </c>
-      <c r="G262" s="15" t="n">
-        <v>3110</v>
-      </c>
-      <c r="H262" s="15" t="s">
-        <v>283</v>
-      </c>
-      <c r="I262" s="15"/>
+        <v>5000</v>
+      </c>
+      <c r="D262" s="13" t="s">
+        <v>199</v>
+      </c>
+      <c r="E262" s="13"/>
+      <c r="F262" s="13"/>
+      <c r="I262" s="13"/>
       <c r="K262" s="1" t="s">
         <v>268</v>
       </c>
@@ -9080,24 +9106,13 @@
         <v>195</v>
       </c>
       <c r="C263" s="13" t="n">
-        <v>3000</v>
-      </c>
-      <c r="D263" s="15" t="s">
-        <v>280</v>
-      </c>
-      <c r="E263" s="15" t="n">
-        <v>3100</v>
-      </c>
-      <c r="F263" s="15" t="s">
-        <v>282</v>
-      </c>
-      <c r="G263" s="15" t="n">
-        <v>3120</v>
-      </c>
-      <c r="H263" s="15" t="s">
-        <v>272</v>
-      </c>
-      <c r="I263" s="15"/>
+        <v>6000</v>
+      </c>
+      <c r="D263" s="13" t="s">
+        <v>203</v>
+      </c>
+      <c r="E263" s="13"/>
+      <c r="I263" s="13"/>
       <c r="K263" s="1" t="s">
         <v>268</v>
       </c>
@@ -9110,120 +9125,120 @@
         <v>195</v>
       </c>
       <c r="C264" s="13" t="n">
-        <v>3000</v>
-      </c>
-      <c r="D264" s="15" t="s">
-        <v>280</v>
-      </c>
-      <c r="E264" s="15" t="n">
-        <v>3100</v>
-      </c>
-      <c r="F264" s="15" t="s">
+        <v>6000</v>
+      </c>
+      <c r="D264" s="13" t="s">
+        <v>203</v>
+      </c>
+      <c r="E264" s="13" t="n">
+        <v>6100</v>
+      </c>
+      <c r="F264" s="13" t="s">
         <v>282</v>
       </c>
-      <c r="G264" s="15" t="n">
-        <v>3130</v>
-      </c>
-      <c r="H264" s="15" t="s">
-        <v>284</v>
-      </c>
-      <c r="I264" s="15"/>
+      <c r="I264" s="13"/>
       <c r="K264" s="1" t="s">
         <v>268</v>
       </c>
     </row>
     <row r="265" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A265" s="13" t="s">
-        <v>264</v>
+        <v>199</v>
       </c>
       <c r="B265" s="13" t="s">
         <v>195</v>
       </c>
       <c r="C265" s="13" t="n">
-        <v>3000</v>
-      </c>
-      <c r="D265" s="15" t="s">
-        <v>280</v>
-      </c>
-      <c r="E265" s="15" t="n">
-        <v>3100</v>
-      </c>
-      <c r="F265" s="15" t="s">
-        <v>282</v>
-      </c>
-      <c r="G265" s="15" t="n">
-        <v>3140</v>
-      </c>
-      <c r="H265" s="15" t="s">
-        <v>285</v>
-      </c>
-      <c r="I265" s="15"/>
+        <v>1000</v>
+      </c>
+      <c r="D265" s="13" t="s">
+        <v>213</v>
+      </c>
+      <c r="E265" s="13"/>
+      <c r="F265" s="13"/>
+      <c r="G265" s="13"/>
+      <c r="H265" s="13"/>
+      <c r="I265" s="13"/>
       <c r="K265" s="1" t="s">
-        <v>268</v>
+        <v>283</v>
       </c>
     </row>
     <row r="266" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A266" s="13" t="s">
-        <v>264</v>
+        <v>199</v>
       </c>
       <c r="B266" s="13" t="s">
         <v>195</v>
       </c>
       <c r="C266" s="13" t="n">
-        <v>5000</v>
+        <v>1000</v>
       </c>
       <c r="D266" s="13" t="s">
-        <v>199</v>
-      </c>
-      <c r="E266" s="13"/>
-      <c r="F266" s="13"/>
+        <v>213</v>
+      </c>
+      <c r="E266" s="13" t="n">
+        <v>1200</v>
+      </c>
+      <c r="F266" s="13" t="s">
+        <v>245</v>
+      </c>
+      <c r="G266" s="13"/>
+      <c r="H266" s="13"/>
       <c r="I266" s="13"/>
       <c r="K266" s="1" t="s">
-        <v>268</v>
+        <v>283</v>
       </c>
     </row>
     <row r="267" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A267" s="13" t="s">
-        <v>264</v>
+        <v>199</v>
       </c>
       <c r="B267" s="13" t="s">
         <v>195</v>
       </c>
       <c r="C267" s="13" t="n">
-        <v>6000</v>
+        <v>1000</v>
       </c>
       <c r="D267" s="13" t="s">
-        <v>203</v>
-      </c>
-      <c r="E267" s="13"/>
-      <c r="F267" s="0"/>
+        <v>213</v>
+      </c>
+      <c r="E267" s="13" t="n">
+        <v>1200</v>
+      </c>
+      <c r="F267" s="13" t="s">
+        <v>245</v>
+      </c>
+      <c r="G267" s="13" t="n">
+        <v>1299</v>
+      </c>
+      <c r="H267" s="13" t="s">
+        <v>246</v>
+      </c>
       <c r="I267" s="13"/>
       <c r="K267" s="1" t="s">
-        <v>268</v>
+        <v>283</v>
       </c>
     </row>
     <row r="268" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A268" s="13" t="s">
-        <v>264</v>
+        <v>199</v>
       </c>
       <c r="B268" s="13" t="s">
         <v>195</v>
       </c>
       <c r="C268" s="13" t="n">
-        <v>6000</v>
+        <v>2000</v>
       </c>
       <c r="D268" s="13" t="s">
         <v>203</v>
       </c>
-      <c r="E268" s="13" t="n">
-        <v>6100</v>
-      </c>
-      <c r="F268" s="16" t="s">
-        <v>286</v>
-      </c>
+      <c r="E268" s="13"/>
+      <c r="F268" s="13"/>
+      <c r="G268" s="13"/>
+      <c r="H268" s="13"/>
       <c r="I268" s="13"/>
       <c r="K268" s="1" t="s">
-        <v>268</v>
+        <v>284</v>
       </c>
     </row>
     <row r="269" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9234,18 +9249,22 @@
         <v>195</v>
       </c>
       <c r="C269" s="13" t="n">
-        <v>1000</v>
+        <v>2000</v>
       </c>
       <c r="D269" s="13" t="s">
-        <v>213</v>
-      </c>
-      <c r="E269" s="13"/>
-      <c r="F269" s="13"/>
+        <v>203</v>
+      </c>
+      <c r="E269" s="13" t="n">
+        <v>2100</v>
+      </c>
+      <c r="F269" s="13" t="s">
+        <v>285</v>
+      </c>
       <c r="G269" s="13"/>
       <c r="H269" s="13"/>
       <c r="I269" s="13"/>
       <c r="K269" s="1" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
     </row>
     <row r="270" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9256,22 +9275,18 @@
         <v>195</v>
       </c>
       <c r="C270" s="13" t="n">
-        <v>1000</v>
-      </c>
-      <c r="D270" s="13" t="s">
-        <v>213</v>
-      </c>
-      <c r="E270" s="13" t="n">
-        <v>1200</v>
-      </c>
-      <c r="F270" s="13" t="s">
-        <v>245</v>
-      </c>
-      <c r="G270" s="13"/>
-      <c r="H270" s="13"/>
-      <c r="I270" s="13"/>
+        <v>3000</v>
+      </c>
+      <c r="D270" s="15" t="s">
+        <v>276</v>
+      </c>
+      <c r="E270" s="15"/>
+      <c r="F270" s="15"/>
+      <c r="G270" s="15"/>
+      <c r="H270" s="15"/>
+      <c r="I270" s="15"/>
       <c r="K270" s="1" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
     </row>
     <row r="271" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9282,26 +9297,22 @@
         <v>195</v>
       </c>
       <c r="C271" s="13" t="n">
-        <v>1000</v>
-      </c>
-      <c r="D271" s="13" t="s">
-        <v>213</v>
-      </c>
-      <c r="E271" s="13" t="n">
-        <v>1200</v>
-      </c>
-      <c r="F271" s="13" t="s">
-        <v>245</v>
-      </c>
-      <c r="G271" s="13" t="n">
-        <v>1299</v>
-      </c>
-      <c r="H271" s="13" t="s">
-        <v>246</v>
-      </c>
-      <c r="I271" s="13"/>
+        <v>3000</v>
+      </c>
+      <c r="D271" s="15" t="s">
+        <v>276</v>
+      </c>
+      <c r="E271" s="15" t="n">
+        <v>3100</v>
+      </c>
+      <c r="F271" s="15" t="s">
+        <v>278</v>
+      </c>
+      <c r="G271" s="15"/>
+      <c r="H271" s="15"/>
+      <c r="I271" s="15"/>
       <c r="K271" s="1" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
     </row>
     <row r="272" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9312,18 +9323,26 @@
         <v>195</v>
       </c>
       <c r="C272" s="13" t="n">
-        <v>2000</v>
-      </c>
-      <c r="D272" s="13" t="s">
-        <v>203</v>
-      </c>
-      <c r="E272" s="13"/>
-      <c r="F272" s="13"/>
-      <c r="G272" s="13"/>
-      <c r="H272" s="13"/>
-      <c r="I272" s="13"/>
+        <v>3000</v>
+      </c>
+      <c r="D272" s="15" t="s">
+        <v>276</v>
+      </c>
+      <c r="E272" s="15" t="n">
+        <v>3100</v>
+      </c>
+      <c r="F272" s="15" t="s">
+        <v>278</v>
+      </c>
+      <c r="G272" s="15" t="n">
+        <v>3120</v>
+      </c>
+      <c r="H272" s="15" t="s">
+        <v>272</v>
+      </c>
+      <c r="I272" s="15"/>
       <c r="K272" s="1" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
     </row>
     <row r="273" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9334,22 +9353,16 @@
         <v>195</v>
       </c>
       <c r="C273" s="13" t="n">
-        <v>2000</v>
+        <v>4000</v>
       </c>
       <c r="D273" s="13" t="s">
-        <v>203</v>
-      </c>
-      <c r="E273" s="13" t="n">
-        <v>2100</v>
-      </c>
-      <c r="F273" s="13" t="s">
-        <v>289</v>
-      </c>
-      <c r="G273" s="13"/>
-      <c r="H273" s="13"/>
+        <v>199</v>
+      </c>
+      <c r="E273" s="13"/>
+      <c r="F273" s="13"/>
       <c r="I273" s="13"/>
       <c r="K273" s="1" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
     </row>
     <row r="274" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9360,18 +9373,16 @@
         <v>195</v>
       </c>
       <c r="C274" s="13" t="n">
-        <v>3000</v>
-      </c>
-      <c r="D274" s="15" t="s">
-        <v>280</v>
-      </c>
-      <c r="E274" s="15"/>
-      <c r="F274" s="15"/>
-      <c r="G274" s="15"/>
-      <c r="H274" s="15"/>
-      <c r="I274" s="15"/>
+        <v>5000</v>
+      </c>
+      <c r="D274" s="13" t="s">
+        <v>197</v>
+      </c>
+      <c r="E274" s="13"/>
+      <c r="F274" s="13"/>
+      <c r="I274" s="13"/>
       <c r="K274" s="1" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
     </row>
     <row r="275" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9382,22 +9393,20 @@
         <v>195</v>
       </c>
       <c r="C275" s="13" t="n">
-        <v>3000</v>
-      </c>
-      <c r="D275" s="15" t="s">
-        <v>280</v>
-      </c>
-      <c r="E275" s="15" t="n">
-        <v>3100</v>
-      </c>
-      <c r="F275" s="15" t="s">
-        <v>282</v>
-      </c>
-      <c r="G275" s="15"/>
-      <c r="H275" s="15"/>
-      <c r="I275" s="15"/>
+        <v>5000</v>
+      </c>
+      <c r="D275" s="13" t="s">
+        <v>197</v>
+      </c>
+      <c r="E275" s="13" t="n">
+        <v>5200</v>
+      </c>
+      <c r="F275" s="13" t="s">
+        <v>247</v>
+      </c>
+      <c r="I275" s="13"/>
       <c r="K275" s="1" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
     </row>
     <row r="276" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9408,26 +9417,20 @@
         <v>195</v>
       </c>
       <c r="C276" s="13" t="n">
-        <v>3000</v>
-      </c>
-      <c r="D276" s="15" t="s">
-        <v>280</v>
-      </c>
-      <c r="E276" s="15" t="n">
-        <v>3100</v>
-      </c>
-      <c r="F276" s="15" t="s">
-        <v>282</v>
-      </c>
-      <c r="G276" s="15" t="n">
-        <v>3120</v>
-      </c>
-      <c r="H276" s="15" t="s">
-        <v>272</v>
-      </c>
-      <c r="I276" s="15"/>
+        <v>5000</v>
+      </c>
+      <c r="D276" s="13" t="s">
+        <v>197</v>
+      </c>
+      <c r="E276" s="13" t="n">
+        <v>5300</v>
+      </c>
+      <c r="F276" s="13" t="s">
+        <v>286</v>
+      </c>
+      <c r="I276" s="13"/>
       <c r="K276" s="1" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
     </row>
     <row r="277" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9438,17 +9441,13 @@
         <v>195</v>
       </c>
       <c r="C277" s="13" t="n">
-        <v>4000</v>
+        <v>6000</v>
       </c>
       <c r="D277" s="13" t="s">
-        <v>199</v>
+        <v>287</v>
       </c>
       <c r="E277" s="13"/>
       <c r="F277" s="13"/>
-      <c r="I277" s="13"/>
-      <c r="K277" s="1" t="s">
-        <v>288</v>
-      </c>
     </row>
     <row r="278" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A278" s="13" t="s">
@@ -9458,16 +9457,16 @@
         <v>195</v>
       </c>
       <c r="C278" s="13" t="n">
-        <v>5000</v>
+        <v>6000</v>
       </c>
       <c r="D278" s="13" t="s">
-        <v>197</v>
-      </c>
-      <c r="E278" s="13"/>
-      <c r="F278" s="13"/>
-      <c r="I278" s="13"/>
-      <c r="K278" s="1" t="s">
         <v>287</v>
+      </c>
+      <c r="E278" s="13" t="n">
+        <v>6100</v>
+      </c>
+      <c r="F278" s="13" t="s">
+        <v>288</v>
       </c>
     </row>
     <row r="279" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9478,20 +9477,16 @@
         <v>195</v>
       </c>
       <c r="C279" s="13" t="n">
-        <v>5000</v>
+        <v>6000</v>
       </c>
       <c r="D279" s="13" t="s">
-        <v>197</v>
+        <v>287</v>
       </c>
       <c r="E279" s="13" t="n">
-        <v>5200</v>
+        <v>6200</v>
       </c>
       <c r="F279" s="13" t="s">
-        <v>247</v>
-      </c>
-      <c r="I279" s="13"/>
-      <c r="K279" s="1" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
     </row>
     <row r="280" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9502,42 +9497,22 @@
         <v>195</v>
       </c>
       <c r="C280" s="13" t="n">
-        <v>5000</v>
+        <v>6000</v>
       </c>
       <c r="D280" s="13" t="s">
-        <v>197</v>
+        <v>287</v>
       </c>
       <c r="E280" s="13" t="n">
-        <v>5300</v>
+        <v>6300</v>
       </c>
       <c r="F280" s="13" t="s">
         <v>290</v>
       </c>
-      <c r="I280" s="13"/>
-      <c r="K280" s="1" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="281" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A281" s="0"/>
-      <c r="B281" s="0"/>
-      <c r="C281" s="0"/>
-      <c r="D281" s="0"/>
-      <c r="E281" s="0"/>
-      <c r="F281" s="0"/>
-      <c r="G281" s="0"/>
-      <c r="H281" s="0"/>
-    </row>
-    <row r="282" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A282" s="0"/>
-      <c r="B282" s="0"/>
-      <c r="C282" s="0"/>
-      <c r="D282" s="0"/>
-      <c r="E282" s="0"/>
-      <c r="F282" s="0"/>
-      <c r="G282" s="0"/>
-      <c r="H282" s="0"/>
-    </row>
+    </row>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>